<commit_message>
insert oracle date string
</commit_message>
<xml_diff>
--- a/xls/schema/data/gameAdmin1.xlsx
+++ b/xls/schema/data/gameAdmin1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="4540" windowWidth="19340" windowHeight="13420"/>
+    <workbookView xWindow="420" yWindow="3980" windowWidth="19340" windowHeight="13420" tabRatio="454"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>出生点面向</t>
   </si>
@@ -316,12 +316,27 @@
     <t>EOF</t>
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>日期</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>2/3/2016  4:27:00 PM</t>
+  </si>
+  <si>
+    <t>3/3/2016  2:27:00 AM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,6 +558,29 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="35">
@@ -854,7 +892,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -982,8 +1020,12 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1022,8 +1064,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="22" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="26" builtinId="38" customBuiltin="1"/>
@@ -1052,11 +1096,15 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="15" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1369,10 +1417,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1382,9 +1430,10 @@
     <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1418,8 +1467,11 @@
       <c r="K1" t="s">
         <v>31</v>
       </c>
+      <c r="L1" s="14" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1450,8 +1502,11 @@
       <c r="K2" t="s">
         <v>25</v>
       </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1485,8 +1540,11 @@
       <c r="K3" t="s">
         <v>34</v>
       </c>
+      <c r="L3" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1520,8 +1578,11 @@
       <c r="K4" s="11">
         <v>0</v>
       </c>
+      <c r="L4" s="15" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1555,8 +1616,11 @@
       <c r="K5" s="11">
         <v>708</v>
       </c>
+      <c r="L5" s="15" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1590,8 +1654,11 @@
       <c r="K6" s="11">
         <v>-1634</v>
       </c>
+      <c r="L6" s="15" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1607,6 +1674,7 @@
   </sheetData>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
xls cell could be empty
</commit_message>
<xml_diff>
--- a/xls/schema/data/gameAdmin1.xlsx
+++ b/xls/schema/data/gameAdmin1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="3980" windowWidth="19340" windowHeight="13420" tabRatio="454"/>
+    <workbookView xWindow="2940" yWindow="2640" windowWidth="21280" windowHeight="14080" tabRatio="340"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="2" r:id="rId1"/>
@@ -329,7 +329,7 @@
     <t>2/3/2016  4:27:00 PM</t>
   </si>
   <si>
-    <t>3/3/2016  2:27:00 AM</t>
+    <t>1/3/2017  2:27:00 AM</t>
   </si>
 </sst>
 </file>
@@ -1419,8 +1419,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1674,7 +1674,6 @@
   </sheetData>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>